<commit_message>
updated notebooks for workshop
</commit_message>
<xml_diff>
--- a/gct/Impacts and pressures.xlsx
+++ b/gct/Impacts and pressures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rml2/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9927D7FB-F712-8243-B4D3-BD54E0FBCB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50A50FB-E081-974C-9618-E55F3AD4CD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="31200" windowHeight="20140" xr2:uid="{00A82159-9831-4BD2-A2D1-4A5A7DDBA21A}"/>
+    <workbookView xWindow="120" yWindow="760" windowWidth="19240" windowHeight="19880" xr2:uid="{00A82159-9831-4BD2-A2D1-4A5A7DDBA21A}"/>
   </bookViews>
   <sheets>
     <sheet name="Australia" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19908" uniqueCount="1732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19918" uniqueCount="1732">
   <si>
     <t>IP_ID</t>
   </si>
@@ -5845,9 +5845,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BU251"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BH154" sqref="BH154"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB226" sqref="AB226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27048,19 +27048,19 @@
         <v xml:space="preserve">Deposition is the laying down of sediment carried by wind, water, or ice. </v>
       </c>
       <c r="V228" s="7">
-        <v>111220</v>
-      </c>
-      <c r="W228" s="7">
-        <v>112220</v>
-      </c>
-      <c r="X228" s="7">
-        <v>123220</v>
-      </c>
-      <c r="Y228" s="7">
-        <v>124220</v>
-      </c>
-      <c r="AA228" s="7">
-        <v>216220</v>
+        <v>220220</v>
+      </c>
+      <c r="W228" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="X228" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="Y228" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="AA228" s="7" t="s">
+        <v>714</v>
       </c>
       <c r="AE228" s="5">
         <v>0</v>
@@ -27094,6 +27094,21 @@
       </c>
       <c r="BD228" s="5">
         <v>2</v>
+      </c>
+      <c r="BJ228" s="5">
+        <v>17</v>
+      </c>
+      <c r="BK228" s="5">
+        <v>18</v>
+      </c>
+      <c r="BL228" s="5">
+        <v>19</v>
+      </c>
+      <c r="BM228" s="5">
+        <v>78</v>
+      </c>
+      <c r="BN228" s="5">
+        <v>89</v>
       </c>
       <c r="BQ228" s="8"/>
       <c r="BR228" s="8"/>
@@ -27152,20 +27167,20 @@
         <f>VLOOKUP(E229,Pressures!$A$2:$B$145,2,FALSE)</f>
         <v>Water changing from a liquid to a gas.</v>
       </c>
-      <c r="V229" s="7">
-        <v>111220</v>
-      </c>
-      <c r="W229" s="7">
-        <v>112220</v>
-      </c>
-      <c r="X229" s="7">
-        <v>123220</v>
-      </c>
-      <c r="Y229" s="7">
-        <v>124220</v>
-      </c>
-      <c r="AA229" s="7">
-        <v>216220</v>
+      <c r="V229" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="W229" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="X229" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="Y229" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="AA229" s="7" t="s">
+        <v>714</v>
       </c>
       <c r="AE229" s="5">
         <v>0</v>
@@ -27310,6 +27325,9 @@
       <c r="P231" s="5" t="str">
         <f>VLOOKUP(E231,Pressures!$A$2:$B$145,2,FALSE)</f>
         <v>Removing silt and other material from the bottom of bodies of water</v>
+      </c>
+      <c r="V231" s="5" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="232" spans="1:71" s="5" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>